<commit_message>
Changes for doc_is and chamber_id continues..
</commit_message>
<xml_diff>
--- a/release/Requirements.xlsx
+++ b/release/Requirements.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -212,6 +212,15 @@
                                                 WHERE a.patient_id = '$patient_id'
                                                 AND a.visited = 'yes' and a.chamber_id='$chamber_name' AND a.doc_id='$doc_name') 
             and b.chamber_id='$chamber_name' AND b.doc_id='$doc_name' ) and c.chamber_id='$chamber_name' AND c.doc_id='$doc_name'</t>
+  </si>
+  <si>
+    <t>Investigation List</t>
+  </si>
+  <si>
+    <t>select a.investigation_name ,  a.ID  from  investigation_master a where a.investigation_name LIKE '$q%' and STATUS = 'ACTIVE' AND a.chamber_id='$chamber_name' AND a.doc_id='$doc_name'</t>
+  </si>
+  <si>
+    <t>select a.investigation_name ,  a.ID  from  investigation_master a where a.investigation_name LIKE 'FB%' and STATUS = 'ACTIVE' AND a.chamber_id='sos' AND a.doc_id='sroy'</t>
   </si>
 </sst>
 </file>
@@ -805,10 +814,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -893,6 +902,29 @@
         <v>46</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed ajax files with modified sql statements
</commit_message>
<xml_diff>
--- a/release/Requirements.xlsx
+++ b/release/Requirements.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -221,6 +221,37 @@
   </si>
   <si>
     <t>select a.investigation_name ,  a.ID  from  investigation_master a where a.investigation_name LIKE 'FB%' and STATUS = 'ACTIVE' AND a.chamber_id='sos' AND a.doc_id='sroy'</t>
+  </si>
+  <si>
+    <t>Get the Investigation list by prescription and visit</t>
+  </si>
+  <si>
+    <t>SELECT b.investigation_name, a.value, b.unit, investigation_id
+                    FROM patient_investigation a, investigation_master b
+                    WHERE a.patient_id = '123'
+                    AND a.visit_id = '10404'
+                    AND a.investigation_id = b.ID and a.chamber_id=b.chamber_id and a.doc_id=b.doc_id and
+     a.chamber_id='sos' AND a.doc_id='sroy'</t>
+  </si>
+  <si>
+    <t>SELECT b.investigation_name, a.value, b.unit, investigation_id
+            FROM patient_investigation a, investigation_master b
+            WHERE a.patient_id = '$patient_id'
+            AND a.visit_id = '$visit_id'
+            AND a.investigation_id = b.ID and a.chamber_id=b.chamber_id and a.doc_id=b.doc_id and
+            a.chamber_id='".$chamber_name."' AND a.doc_id='".$doc_name."'</t>
+  </si>
+  <si>
+    <t>SELECT b.type, b.ID
+                        FROM prescribed_cf a, clinical_impression b
+                        WHERE a.clinical_impression_id = b.id and a.chamber_id=b.chamber_id and a.doc_id=b.doc_id and
+                        AND a.prescription_id = '$PRESCRIPTION_ID' and a.chamber_id='".$chamber_name."' AND a.doc_id='".$doc_name."'</t>
+  </si>
+  <si>
+    <t>Clinical impression List by prescription</t>
+  </si>
+  <si>
+    <t>makeprescription/clinical_impression.php</t>
   </si>
 </sst>
 </file>
@@ -814,116 +845,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="112.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="112.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="83.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="165" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="165" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2.1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="180" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:5" ht="180" x14ac:dyDescent="0.35">
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.35">
+      <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="2"/>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.35">
+      <c r="B11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed ajax files with modified sql statements-Continued
</commit_message>
<xml_diff>
--- a/release/Requirements.xlsx
+++ b/release/Requirements.xlsx
@@ -242,16 +242,16 @@
             a.chamber_id='".$chamber_name."' AND a.doc_id='".$doc_name."'</t>
   </si>
   <si>
+    <t>Clinical impression List by prescription</t>
+  </si>
+  <si>
+    <t>makeprescription/clinical_impression.php</t>
+  </si>
+  <si>
     <t>SELECT b.type, b.ID
                         FROM prescribed_cf a, clinical_impression b
-                        WHERE a.clinical_impression_id = b.id and a.chamber_id=b.chamber_id and a.doc_id=b.doc_id and
+                        WHERE a.clinical_impression_id = b.id and a.chamber_id=b.chamber_id and a.doc_id=b.doc_id
                         AND a.prescription_id = '$PRESCRIPTION_ID' and a.chamber_id='".$chamber_name."' AND a.doc_id='".$doc_name."'</t>
-  </si>
-  <si>
-    <t>Clinical impression List by prescription</t>
-  </si>
-  <si>
-    <t>makeprescription/clinical_impression.php</t>
   </si>
 </sst>
 </file>
@@ -848,7 +848,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
@@ -958,13 +958,13 @@
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Commiting the changes for testing
</commit_message>
<xml_diff>
--- a/release/Requirements.xlsx
+++ b/release/Requirements.xlsx
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>

</xml_diff>